<commit_message>
Add moderator model and encode forum posts in utf-8
</commit_message>
<xml_diff>
--- a/DataSet.xlsx
+++ b/DataSet.xlsx
@@ -5340,8 +5340,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A931" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E931" activeCellId="0" sqref="E931"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A635" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B635" activeCellId="0" sqref="B635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9620,7 +9620,7 @@
         <v>521</v>
       </c>
       <c r="B535" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9628,7 +9628,7 @@
         <v>522</v>
       </c>
       <c r="B536" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add tests for models
</commit_message>
<xml_diff>
--- a/DataSet.xlsx
+++ b/DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="918">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -5201,6 +5201,13 @@
 &lt;div class="centerBoxContentsFeatured centeredContent back" style="width:33%;"&gt;&lt;a href="http://www.watches24shop.top/it/copia-orologi-rolex-gmt-master-orologio-ref-1675-vintage-edition-nero-lunetta-stesso-telaio-come-swiss-eta-versi-post4030-313b-p-510.html"&gt;&lt;div style="vertical-align: middle;height:150px"&gt;&lt;img src="http://it.watches24shop.top/images/_small//watches_11/Rolex/Replica-Rolex-Gmt-Master-Watch-Ref-1675-Vintage.jpg" alt="Copia Orologi Rolex Gmt Master Orologio Ref. 1675 Vintage Edition Nero Lunetta Stesso telaio, come Swiss Eta Versi Post4030 [313b]" title=" Copia Orologi Rolex Gmt Master Orologio Ref. 1675 Vintage Edition Nero Lunetta Stesso telaio, come Swiss Eta Versi Post4030 [313b] " width="200" height="150" /&gt;&lt;/div&gt;&lt;/a&gt;&lt;br /&gt;&lt;a href="http://www.watches24shop.top/it/copia-orologi-rolex-gmt-master-orologio-ref-1675-vintage-edition-nero-lunetta-stesso-telaio-come-swiss-eta-versi-post4030-313b-p-510.html"&gt;Copia Orologi Rolex Gmt Master Orologio Ref. 1675 Vintage Edition Nero Lunetta Stesso telaio, come Swiss Eta Versi Post4030 [313b]&lt;/a&gt;&lt;br /&gt;&lt;span class="normalprice"&gt;&amp;euro;920.70 &lt;/span&gt; &lt;span class="productSpecialPrice"&gt;&amp;euro;195.30&lt;/span&gt;&lt;span class="productPriceDiscount"&gt;&lt;br /&gt;Risparmi: 79% sconto&lt;/span&gt;&lt;/div&gt;
 &lt;br class="clearBoth" /&gt;&lt;div class="centerBoxContentsFeatured centeredContent back" style="width:33%;"&gt;&lt;a href="http://www.watches24shop.top/it/copia-orologi-rolex-gmt-master-orologio-ref-1675-case-nero-vintage-edition</t>
   </si>
+  <si>
+    <t xml:space="preserve">Now I'm not usually one to get annoyed about the length of time it takes to figure something out, afterall this is touchdesigner, however I can't help but get frustrated at python third party modules and how I'm supposed to get them working.Lets begin at this weeks challenge, simple enough, getting twitters 1.1 api to work with touchdesigner via python.So it turns out the new twitter API demands SSL, it's not a recommendation but an actual requirement of the 1.1 api which I'm beginning to dislike more and more. So I get a no ssl module error which I find odd as I can see the ssl module file in my touchdesigner installation and after a bit of googling it turns out that you need to compile python with ssl support...which leads to the final problem...I can't just go recompiling the python installation in my touchdesigner directory? Please help, I didn’t find the right solution from the internet. &lt;a href=””&gt;Video&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The laptop in question is an Inspiron 1545. It's running Windows 7.When it's powered on, the screen is either black, though back-lit, black with vertical white stripes on roughly a fifth of the screen, or black with white as well as thinner, colored stripes vertically, still on about a fifth of the screen. It won't progress to the Windows start page. Trying to get it to start in safe mode doesn't do anything. It has a VGA out, but when I plugged it into an external monitor, it won't actually output to the monitor. I'm thinking it's either a driver issue or a connection issue. Any advice?Please help.I did not find the right solution from the internet.References:https://arstechnica.com/civis/viewtopic.php?f=6&amp;t=1170367
+&lt;a href=””&gt;Video production quote&lt;/a&gt; Thanks!</t>
+  </si>
 </sst>
 </file>
 
@@ -5340,8 +5347,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A635" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B635" activeCellId="0" sqref="B635"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A936" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A936" activeCellId="0" sqref="A936"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12811,7 +12818,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A935" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="B935" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="936" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A936" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="B936" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A103" r:id="rId1" display="http://forums.fossee.in/question/31/while-creating-up-counter-block-in-python-getting-following-erros-at-cmake/"/>

</xml_diff>

<commit_message>
Embed CKEditor in question/answer body
</commit_message>
<xml_diff>
--- a/DataSet.xlsx
+++ b/DataSet.xlsx
@@ -4787,13 +4787,13 @@
     <t xml:space="preserve">While simulating the circuit we get "error while opening python plot editor" , we tried a lot. I think I can get the better solution from u for this problem.</t>
   </si>
   <si>
-    <t xml:space="preserve">Lussuoso Rolex Replica Watches, orologi replica migliore qualità svizzera in vendita online! &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Replica Watches, I migliori falsi orologi in vendita, orologi &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Migliori Swiss Replica Watches Hublot alta qualità , facilmente acquistare le imitazioni perfette di orologi Hublot . &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt;</t>
+    <t xml:space="preserve">Lussuoso Rolex Replica Watches, orologi replica migliore qualità svizzera in vendita online! &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replica Watches, I migliori falsi orologi in vendita, orologi &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Migliori Swiss Replica Watches Hublot alta qualità , facilmente acquistare le imitazioni perfette di orologi Hublot . &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">TAG Heuer watches &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;img /&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt; &lt;a href=””&gt;</t>
@@ -5347,8 +5347,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A936" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A936" activeCellId="0" sqref="A936"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A926" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A929" activeCellId="0" sqref="A929"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12754,7 +12754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="927" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="927" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A927" s="4" t="s">
         <v>908</v>
       </c>
@@ -12762,7 +12762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="928" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="928" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A928" s="4" t="s">
         <v>909</v>
       </c>
@@ -12770,7 +12770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="929" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="929" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A929" s="4" t="s">
         <v>910</v>
       </c>

</xml_diff>